<commit_message>
Moving datasources outside project structure
</commit_message>
<xml_diff>
--- a/configurations/experiment_configs_liver.xlsx
+++ b/configurations/experiment_configs_liver.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="186" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="122">
   <si>
     <t xml:space="preserve">var_name</t>
   </si>
@@ -388,6 +388,9 @@
   </si>
   <si>
     <t xml:space="preserve">lm_groups</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.8,.8,1.5</t>
   </si>
 </sst>
 </file>
@@ -524,7 +527,7 @@
   <dimension ref="A1:I1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="4:4 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -881,7 +884,7 @@
   <dimension ref="A1:K26"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A12" activeCellId="1" sqref="4:4 A12"/>
+      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1181,7 +1184,7 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G7" activeCellId="1" sqref="4:4 G7"/>
+      <selection pane="topLeft" activeCell="G7" activeCellId="0" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1431,7 +1434,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E7" activeCellId="1" sqref="4:4 E7"/>
+      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1567,7 +1570,7 @@
   <dimension ref="A1:F1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A7" activeCellId="1" sqref="4:4 A7"/>
+      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1675,10 +1678,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="4:4"/>
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.15234375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1720,6 +1723,14 @@
         <v>120</v>
       </c>
     </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>121</v>
+      </c>
+    </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
BBox transforms in detection file. Next iteration will have bbox drawn after all image tfms
</commit_message>
<xml_diff>
--- a/configurations/experiment_configs_liver.xlsx
+++ b/configurations/experiment_configs_liver.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="7"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="model_params" sheetId="1" state="visible" r:id="rId2"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="125">
   <si>
     <t xml:space="preserve">var_name</t>
   </si>
@@ -224,6 +224,15 @@
     <t xml:space="preserve">[0,1.]</t>
   </si>
   <si>
+    <t xml:space="preserve">cache_rate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ds_type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">None</t>
+  </si>
+  <si>
     <t xml:space="preserve">plan</t>
   </si>
   <si>
@@ -339,9 +348,6 @@
   </si>
   <si>
     <t xml:space="preserve">ce_weight</t>
-  </si>
-  <si>
-    <t xml:space="preserve">None</t>
   </si>
   <si>
     <t xml:space="preserve">lambda_ce</t>
@@ -539,7 +545,7 @@
       <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.19140625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.2109375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="33.83"/>
@@ -892,11 +898,11 @@
   </sheetPr>
   <dimension ref="A1:K1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E13" activeCellId="0" sqref="E13"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E14" activeCellId="0" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.19140625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.2109375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.81"/>
@@ -1112,22 +1118,38 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="13" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="2" t="s">
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="s">
         <v>65</v>
       </c>
-      <c r="B13" s="2"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="2" t="n">
+      <c r="B13" s="0" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="D13" s="1"/>
+    </row>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="B14" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="D14" s="1"/>
+    </row>
+    <row r="15" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="B15" s="2"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="2" t="n">
         <v>3</v>
       </c>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="J13" s="2"/>
-    </row>
-    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="J15" s="2"/>
+    </row>
+    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1151,7 +1173,7 @@
       <selection pane="topLeft" activeCell="G7" activeCellId="0" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.19140625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.2109375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.38"/>
@@ -1171,13 +1193,13 @@
         <v>2</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
       <c r="E1" s="0" t="s">
         <v>1</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="G1" s="0" t="s">
         <v>4</v>
@@ -1185,119 +1207,119 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="B2" s="1" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="F2" s="0" t="n">
         <v>0.1</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="B3" s="1" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="F3" s="0" t="n">
         <v>0.1</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="B4" s="1" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="F4" s="0" t="n">
         <v>0.1</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="B5" s="1" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="F5" s="0" t="n">
         <v>0.1</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="B6" s="1" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="F6" s="0" t="n">
         <v>0.1</v>
@@ -1308,55 +1330,55 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="B7" s="1" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="F7" s="0" t="n">
         <v>0.1</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="B8" s="1" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="F8" s="0" t="n">
         <v>0.1</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="B9" s="1" t="n">
         <f aca="false">FALSE()</f>
@@ -1366,7 +1388,7 @@
         <v>8</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="E9" s="0" t="s">
         <v>24</v>
@@ -1401,7 +1423,7 @@
       <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.19140625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.2109375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.63"/>
@@ -1427,33 +1449,33 @@
         <v>4</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="D2" s="1" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="D3" s="1" t="n">
         <f aca="false">FALSE()</f>
@@ -1463,30 +1485,30 @@
         <v>0</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="D4" s="1" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="D5" s="1" t="n">
         <f aca="false">FALSE()</f>
@@ -1499,13 +1521,13 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="D6" s="1" t="n">
         <f aca="false">FALSE()</f>
@@ -1537,7 +1559,7 @@
       <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.19140625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.2109375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.33"/>
@@ -1561,24 +1583,24 @@
         <v>4</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="D2" s="1" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>104</v>
+        <v>67</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="D3" s="1"/>
       <c r="E3" s="0" t="n">
@@ -1587,7 +1609,7 @@
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
       <c r="D4" s="1" t="n">
         <f aca="false">FALSE()</f>
@@ -1599,19 +1621,19 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="D5" s="1" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="D6" s="1" t="n">
         <f aca="false">FALSE()</f>
@@ -1648,7 +1670,7 @@
       <selection pane="topLeft" activeCell="H55" activeCellId="0" sqref="H55"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.19140625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.2109375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.76"/>
@@ -1676,28 +1698,28 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>40</v>
@@ -1705,7 +1727,7 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>1</v>
@@ -1713,15 +1735,15 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>0.25</v>
@@ -1729,7 +1751,7 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>0</v>
@@ -1757,7 +1779,7 @@
       <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.18359375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.19140625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="28.57"/>
@@ -1786,28 +1808,28 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>40</v>
@@ -1815,7 +1837,7 @@
     </row>
     <row r="6" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>1</v>
@@ -1831,10 +1853,10 @@
     </row>
     <row r="7" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="C7" s="0"/>
       <c r="D7" s="0"/>
@@ -1863,11 +1885,11 @@
   </sheetPr>
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.18359375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.48"/>
   </cols>
@@ -1894,36 +1916,36 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
Patchbased training new version
</commit_message>
<xml_diff>
--- a/configurations/experiment_configs_liver.xlsx
+++ b/configurations/experiment_configs_liver.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="model_params" sheetId="1" state="visible" r:id="rId2"/>
@@ -16,6 +16,8 @@
     <sheet name="plan1" sheetId="6" state="visible" r:id="rId7"/>
     <sheet name="plan2" sheetId="7" state="visible" r:id="rId8"/>
     <sheet name="plan3" sheetId="8" state="visible" r:id="rId9"/>
+    <sheet name="plan4" sheetId="9" state="visible" r:id="rId10"/>
+    <sheet name="plan5" sheetId="10" state="visible" r:id="rId11"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -27,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="131">
   <si>
     <t xml:space="preserve">var_name</t>
   </si>
@@ -167,241 +169,259 @@
     <t xml:space="preserve">batch_size</t>
   </si>
   <si>
+    <t xml:space="preserve">src_dims</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[192,192,128]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[192,192,96]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[256,256,64]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[160,160,160]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[192,192,160]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[220,220,110]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[256,256,128]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">patch_dim0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[64,96,128,160,256]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">patch_dim1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[48,64,96,128]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fgbg_ratio</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[None,tumour]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[4,2,2,2,2,2]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fake_tumours</t>
+  </si>
+  <si>
+    <t xml:space="preserve">random_sample</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0,1.]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cache_rate</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ds_type</t>
+  </si>
+  <si>
+    <t xml:space="preserve">None</t>
+  </si>
+  <si>
+    <t xml:space="preserve">s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">plan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tune_p</t>
+  </si>
+  <si>
+    <t xml:space="preserve">manual_p</t>
+  </si>
+  <si>
+    <t xml:space="preserve">contrast</t>
+  </si>
+  <si>
+    <t xml:space="preserve">double_range</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.0,1.0]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.25,0.5],[1.5,2.0]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.7,1.3]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">shift</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-1,-0.5],[0.5,1.0]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[-1.0,1.0]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">absolute value shift</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scale</t>
+  </si>
+  <si>
+    <t xml:space="preserve">noise_ub</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0,.25],[.25,.5]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0,.25]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">noise_monai</t>
+  </si>
+  <si>
+    <t xml:space="preserve">range</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.05,.25]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">noise</t>
+  </si>
+  <si>
+    <t xml:space="preserve">brightness</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.5,1.0],[1.0,2.0]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.7,2.0]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">flip</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Notes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rotate_range</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0,0.785]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.20,0.2,0.35]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">translate_factor</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.05,0.15]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">uniform</t>
+  </si>
+  <si>
+    <t xml:space="preserve">translate worsens dice</t>
+  </si>
+  <si>
+    <t xml:space="preserve">scale_range</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.15,0.15,0.15]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">shear</t>
+  </si>
+  <si>
+    <t xml:space="preserve">p</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.,1.]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">notes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ce_weight</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lambda_ce</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lambda_dice</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mean</t>
+  </si>
+  <si>
+    <t xml:space="preserve">softmax</t>
+  </si>
+  <si>
+    <t xml:space="preserve">datasources</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lits,drli,litq,litqsmall</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lm_groups</t>
+  </si>
+  <si>
+    <t xml:space="preserve">spacing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.8,.8,1.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">expand_by_lbd</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fg_indices_exclude</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">patch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">patch_overlap</t>
+  </si>
+  <si>
+    <t xml:space="preserve">expand_by_patch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lbd</t>
+  </si>
+  <si>
     <t xml:space="preserve">samples_per_file</t>
   </si>
   <si>
-    <t xml:space="preserve">src_dims</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[192,192,128]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[192,192,96]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[256,256,64]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[160,160,160]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[192,192,160]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[220,220,110]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[256,256,128]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">patch_dim0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[64,96,128,160,256]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">patch_dim1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[48,64,96,128]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fgbg_ratio</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[None,tumour]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[4,2,2,2,2,2]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fake_tumours</t>
-  </si>
-  <si>
-    <t xml:space="preserve">random_sample</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0,1.]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cache_rate</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ds_type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">None</t>
-  </si>
-  <si>
-    <t xml:space="preserve">plan</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tune_p</t>
-  </si>
-  <si>
-    <t xml:space="preserve">manual_p</t>
-  </si>
-  <si>
-    <t xml:space="preserve">contrast</t>
-  </si>
-  <si>
-    <t xml:space="preserve">double_range</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.0,1.0]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.25,0.5],[1.5,2.0]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.7,1.3]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">shift</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[-1,-0.5],[0.5,1.0]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[-1.0,1.0]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">absolute value shift</t>
-  </si>
-  <si>
-    <t xml:space="preserve">scale</t>
-  </si>
-  <si>
-    <t xml:space="preserve">noise_ub</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0,.25],[.25,.5]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0,.25]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">noise_monai</t>
-  </si>
-  <si>
-    <t xml:space="preserve">range</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.05,.25]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">noise</t>
-  </si>
-  <si>
-    <t xml:space="preserve">brightness</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.5,1.0],[1.0,2.0]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.7,2.0]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">flip</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Notes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rotate_range</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0,0.785]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.20,0.2,0.35]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">translate_factor</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.05,0.15]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">uniform</t>
-  </si>
-  <si>
-    <t xml:space="preserve">translate worsens dice</t>
-  </si>
-  <si>
-    <t xml:space="preserve">scale_range</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.15,0.15,0.15]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">shear</t>
-  </si>
-  <si>
-    <t xml:space="preserve">p</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.,1.]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">notes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ce_weight</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lambda_ce</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lambda_dice</t>
-  </si>
-  <si>
-    <t xml:space="preserve">reduction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mean</t>
-  </si>
-  <si>
-    <t xml:space="preserve">softmax</t>
-  </si>
-  <si>
-    <t xml:space="preserve">datasources</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lits,drli,litq,litqsmall</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lm_groups</t>
-  </si>
-  <si>
-    <t xml:space="preserve">spacing</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.8,.8,1.5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">expand_by_lbd</t>
-  </si>
-  <si>
-    <t xml:space="preserve">fg_indices_exclude</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mode</t>
-  </si>
-  <si>
-    <t xml:space="preserve">patch</t>
-  </si>
-  <si>
-    <t xml:space="preserve">patch_overlap</t>
-  </si>
-  <si>
-    <t xml:space="preserve">expand_by_patch</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lbd</t>
-  </si>
-  <si>
     <t xml:space="preserve">source</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.8,0.8,1.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">patch_size</t>
+  </si>
+  <si>
+    <t xml:space="preserve">320, 320, 192</t>
+  </si>
+  <si>
+    <t xml:space="preserve">source_plan</t>
+  </si>
+  <si>
+    <t xml:space="preserve">plan4</t>
   </si>
 </sst>
 </file>
@@ -545,7 +565,7 @@
       <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.2109375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.33"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="33.83"/>
@@ -891,6 +911,124 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:F15"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.5"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>121</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>0.25</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="s">
+        <v>127</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="B10" s="0" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
   <sheetPr filterMode="false">
@@ -898,11 +1036,11 @@
   </sheetPr>
   <dimension ref="A1:K1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E14" activeCellId="0" sqref="E14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.2109375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="17.83"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.81"/>
@@ -978,7 +1116,7 @@
       </c>
       <c r="D5" s="1"/>
       <c r="E5" s="2" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="F5" s="2"/>
       <c r="G5" s="2"/>
@@ -991,48 +1129,52 @@
         <v>46</v>
       </c>
       <c r="D6" s="1"/>
-      <c r="E6" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
+      <c r="E6" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="K6" s="0" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="D7" s="1"/>
-      <c r="E7" s="2" t="s">
-        <v>48</v>
-      </c>
-      <c r="F7" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="G7" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>51</v>
-      </c>
-      <c r="I7" s="2" t="s">
-        <v>52</v>
-      </c>
-      <c r="J7" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="K7" s="0" t="s">
         <v>54</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>55</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>8</v>
+      </c>
+      <c r="D7" s="1" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="E7" s="2" t="n">
+        <v>128</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C8" s="0" t="s">
         <v>8</v>
@@ -1042,15 +1184,15 @@
         <v>0</v>
       </c>
       <c r="E8" s="2" t="n">
-        <v>128</v>
+        <v>96</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C9" s="0" t="s">
         <v>8</v>
@@ -1059,16 +1201,19 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="E9" s="2" t="n">
-        <v>96</v>
+      <c r="E9" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="I9" s="0" t="s">
+        <v>60</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>60</v>
+        <v>24</v>
       </c>
       <c r="C10" s="0" t="s">
         <v>8</v>
@@ -1077,11 +1222,9 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="E10" s="0" t="n">
-        <v>3</v>
-      </c>
-      <c r="I10" s="0" t="s">
-        <v>61</v>
+      <c r="E10" s="1" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1089,67 +1232,52 @@
         <v>62</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="C11" s="0" t="s">
-        <v>8</v>
+        <v>63</v>
       </c>
       <c r="D11" s="1" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="E11" s="1" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
+      <c r="E11" s="0" t="n">
+        <v>0.5</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>63</v>
-      </c>
-      <c r="B12" s="0" t="s">
         <v>64</v>
       </c>
-      <c r="D12" s="1" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="E12" s="0" t="n">
-        <v>0.5</v>
-      </c>
+      <c r="B12" s="0" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="D12" s="1"/>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
         <v>65</v>
       </c>
-      <c r="B13" s="0" t="n">
-        <v>0.3</v>
+      <c r="B13" s="0" t="s">
+        <v>66</v>
       </c>
       <c r="D13" s="1"/>
-    </row>
-    <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="B14" s="0" t="s">
+      <c r="E13" s="0" t="s">
         <v>67</v>
       </c>
-      <c r="D14" s="1"/>
-    </row>
-    <row r="15" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="2" t="s">
+    </row>
+    <row r="14" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="2" t="s">
         <v>68</v>
       </c>
-      <c r="B15" s="2"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="2" t="n">
-        <v>3</v>
-      </c>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-      <c r="J15" s="2"/>
-    </row>
-    <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="B14" s="2"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="J14" s="2"/>
+    </row>
+    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1173,7 +1301,7 @@
       <selection pane="topLeft" activeCell="G7" activeCellId="0" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.2109375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.265625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.66"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="11.38"/>
@@ -1423,7 +1551,7 @@
       <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.2109375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.63"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.63"/>
@@ -1559,7 +1687,7 @@
       <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.2109375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="14.54"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.33"/>
@@ -1595,7 +1723,7 @@
         <v>0</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1666,11 +1794,11 @@
   </sheetPr>
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H55" activeCellId="0" sqref="H55"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G15" activeCellId="0" sqref="G15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.2109375" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.265625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="27.78"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.76"/>
@@ -1773,13 +1901,13 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J7"/>
+  <dimension ref="A1:J8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.19140625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.25390625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="28.57"/>
@@ -1866,6 +1994,14 @@
       <c r="H7" s="0"/>
       <c r="I7" s="0"/>
       <c r="J7" s="0"/>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>2</v>
+      </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1889,7 +2025,7 @@
       <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.18359375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="9.23828125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.48"/>
   </cols>
@@ -1945,10 +2081,17 @@
         <v>119</v>
       </c>
       <c r="B6" s="0" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="B7" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
@@ -1960,4 +2103,120 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:J8"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.25390625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="28.57"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="25.57"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="0" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="0" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="0" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="0" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="0" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="s">
+        <v>112</v>
+      </c>
+      <c r="B2" s="0" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="s">
+        <v>115</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="s">
+        <v>118</v>
+      </c>
+      <c r="B6" s="0"/>
+      <c r="C6" s="0"/>
+      <c r="D6" s="0"/>
+      <c r="E6" s="0"/>
+      <c r="F6" s="0"/>
+      <c r="G6" s="0"/>
+      <c r="H6" s="0"/>
+      <c r="I6" s="0"/>
+      <c r="J6" s="0"/>
+    </row>
+    <row r="7" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="s">
+        <v>119</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>123</v>
+      </c>
+      <c r="C7" s="0"/>
+      <c r="D7" s="0"/>
+      <c r="E7" s="0"/>
+      <c r="F7" s="0"/>
+      <c r="G7" s="0"/>
+      <c r="H7" s="0"/>
+      <c r="I7" s="0"/>
+      <c r="J7" s="0"/>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
working. various bugs quashed
</commit_message>
<xml_diff>
--- a/configurations/experiment_configs_liver.xlsx
+++ b/configurations/experiment_configs_liver.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="12"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="model_params" sheetId="1" state="visible" r:id="rId3"/>
@@ -21,6 +21,7 @@
     <sheet name="plan6" sheetId="11" state="visible" r:id="rId13"/>
     <sheet name="plan7" sheetId="12" state="visible" r:id="rId14"/>
     <sheet name="plan8" sheetId="13" state="visible" r:id="rId15"/>
+    <sheet name="plantmp" sheetId="14" state="visible" r:id="rId16"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="138">
   <si>
     <t xml:space="preserve">var_name</t>
   </si>
@@ -443,6 +444,9 @@
   </si>
   <si>
     <t xml:space="preserve">plan7</t>
+  </si>
+  <si>
+    <t xml:space="preserve">drli_short</t>
   </si>
 </sst>
 </file>
@@ -1382,8 +1386,8 @@
   </sheetPr>
   <dimension ref="A1:F8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B7" activeCellId="0" sqref="B7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="I57" activeCellId="0" sqref="I57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.16015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1471,6 +1475,119 @@
       <c r="A8" s="1"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;Kffffff&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;KffffffPage &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:F9"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="10.16015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetData>
+    <row r="1" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="C2" s="1"/>
+    </row>
+    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="C3" s="1"/>
+    </row>
+    <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="C4" s="1"/>
+    </row>
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B5" s="1" t="n">
+        <v>40</v>
+      </c>
+      <c r="C5" s="1"/>
+    </row>
+    <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B6" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="C6" s="1"/>
+    </row>
+    <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C7" s="1"/>
+    </row>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="B8" s="1" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="C8" s="1"/>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="B9" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="C9" s="1"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1703,15 +1820,15 @@
       <c r="B12" s="1" t="n">
         <v>0.3</v>
       </c>
-      <c r="C12" s="0"/>
+      <c r="C12" s="1"/>
       <c r="D12" s="2"/>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
-      <c r="H12" s="0"/>
-      <c r="I12" s="0"/>
+      <c r="H12" s="1"/>
+      <c r="I12" s="1"/>
       <c r="J12" s="1"/>
-      <c r="K12" s="0"/>
+      <c r="K12" s="1"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
@@ -2261,12 +2378,13 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G15" activeCellId="0" sqref="G15"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.265625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="27.78"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="15.76"/>
   </cols>
   <sheetData>
@@ -2420,14 +2538,14 @@
       <c r="B4" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="C4" s="0"/>
-      <c r="D4" s="0"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
-      <c r="G4" s="0"/>
-      <c r="H4" s="0"/>
-      <c r="I4" s="0"/>
-      <c r="J4" s="0"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
     </row>
     <row r="5" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
@@ -2436,14 +2554,14 @@
       <c r="B5" s="1" t="n">
         <v>40</v>
       </c>
-      <c r="C5" s="0"/>
-      <c r="D5" s="0"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
-      <c r="G5" s="0"/>
-      <c r="H5" s="0"/>
-      <c r="I5" s="0"/>
-      <c r="J5" s="0"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
@@ -2641,14 +2759,14 @@
       <c r="B4" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="C4" s="0"/>
-      <c r="D4" s="0"/>
+      <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
-      <c r="G4" s="0"/>
-      <c r="H4" s="0"/>
-      <c r="I4" s="0"/>
-      <c r="J4" s="0"/>
+      <c r="G4" s="1"/>
+      <c r="H4" s="1"/>
+      <c r="I4" s="1"/>
+      <c r="J4" s="1"/>
     </row>
     <row r="5" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
@@ -2657,14 +2775,14 @@
       <c r="B5" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="C5" s="0"/>
-      <c r="D5" s="0"/>
+      <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
-      <c r="G5" s="0"/>
-      <c r="H5" s="0"/>
-      <c r="I5" s="0"/>
-      <c r="J5" s="0"/>
+      <c r="G5" s="1"/>
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">

</xml_diff>

<commit_message>
colour palette, whole img infrernce
</commit_message>
<xml_diff>
--- a/configurations/experiment_configs_liver.xlsx
+++ b/configurations/experiment_configs_liver.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="13"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="model_params" sheetId="1" state="visible" r:id="rId3"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="137">
   <si>
     <t xml:space="preserve">var_name</t>
   </si>
@@ -156,9 +156,6 @@
   </si>
   <si>
     <t xml:space="preserve">compiled</t>
-  </si>
-  <si>
-    <t xml:space="preserve">src_dest_labels</t>
   </si>
   <si>
     <t xml:space="preserve">fold</t>
@@ -1080,33 +1077,33 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>112</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>115</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B6" s="1" t="n">
         <v>1</v>
@@ -1114,15 +1111,15 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>119</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B8" s="1" t="n">
         <v>0.25</v>
@@ -1130,18 +1127,18 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>128</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>130</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1199,28 +1196,28 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>112</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>115</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B5" s="1" t="n">
         <v>40</v>
@@ -1228,29 +1225,29 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B6" s="1"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>132</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>133</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B9" s="1" t="n">
         <v>2</v>
@@ -1307,28 +1304,28 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>112</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>115</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B5" s="1" t="n">
         <v>70</v>
@@ -1336,7 +1333,7 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -1348,10 +1345,10 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
@@ -1362,7 +1359,7 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B8" s="1" t="n">
         <v>2</v>
@@ -1414,24 +1411,24 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>112</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>113</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -1441,10 +1438,10 @@
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
@@ -1453,17 +1450,17 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B7" s="1" t="n">
         <v>1</v>
@@ -1494,7 +1491,7 @@
   </sheetPr>
   <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
@@ -1522,31 +1519,31 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C2" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C3" s="1"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>115</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>116</v>
       </c>
       <c r="C4" s="1"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B5" s="1" t="n">
         <v>40</v>
@@ -1555,7 +1552,7 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B6" s="1" t="n">
         <v>1</v>
@@ -1564,16 +1561,16 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>119</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>120</v>
       </c>
       <c r="C7" s="1"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B8" s="1" t="n">
         <v>0.25</v>
@@ -1582,7 +1579,7 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B9" s="1" t="n">
         <v>0</v>
@@ -1607,8 +1604,8 @@
   </sheetPr>
   <dimension ref="A1:K1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E14" activeCellId="0" sqref="E14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1648,35 +1645,37 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="E2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
+      <c r="E2" s="6" t="n">
+        <v>3</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="D3" s="2" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="E3" s="6" t="n">
-        <v>3</v>
-      </c>
+      <c r="D3" s="2"/>
+      <c r="E3" s="7" t="n">
+        <f aca="false">TRUE()</f>
+        <v>1</v>
+      </c>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="D4" s="2"/>
-      <c r="E4" s="7" t="n">
-        <f aca="false">TRUE()</f>
-        <v>1</v>
+      <c r="E4" s="3" t="n">
+        <v>10</v>
       </c>
       <c r="F4" s="3"/>
-      <c r="G4" s="3" t="s">
-        <v>44</v>
-      </c>
+      <c r="G4" s="3"/>
       <c r="H4" s="3"/>
       <c r="I4" s="3"/>
       <c r="J4" s="3"/>
@@ -1686,48 +1685,52 @@
         <v>45</v>
       </c>
       <c r="D5" s="2"/>
-      <c r="E5" s="3" t="n">
-        <v>10</v>
-      </c>
-      <c r="F5" s="3"/>
-      <c r="G5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
+      <c r="E5" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D6" s="2"/>
-      <c r="E6" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="J6" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="K6" s="1" t="s">
         <v>53</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="2" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="E6" s="3" t="n">
+        <v>128</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>8</v>
@@ -1737,15 +1740,15 @@
         <v>0</v>
       </c>
       <c r="E7" s="3" t="n">
-        <v>128</v>
+        <v>96</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>8</v>
@@ -1754,16 +1757,19 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="E8" s="3" t="n">
-        <v>96</v>
+      <c r="E8" s="1" t="n">
+        <v>3</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>59</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>59</v>
+        <v>24</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>8</v>
@@ -1772,11 +1778,9 @@
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="E9" s="1" t="n">
-        <v>3</v>
-      </c>
-      <c r="I9" s="1" t="s">
-        <v>60</v>
+      <c r="E9" s="2" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1784,82 +1788,64 @@
         <v>61</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>8</v>
+        <v>62</v>
       </c>
       <c r="D10" s="2" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
-      <c r="E10" s="2" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E10" s="1" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="11" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="B11" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="D11" s="2" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="E11" s="1" t="n">
-        <v>0.5</v>
-      </c>
-    </row>
-    <row r="12" s="6" customFormat="true" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B11" s="1" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="C11" s="1"/>
+      <c r="D11" s="2"/>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+      <c r="I11" s="1"/>
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="B12" s="1" t="n">
-        <v>0.3</v>
-      </c>
-      <c r="C12" s="1"/>
+      <c r="B12" s="1" t="s">
+        <v>65</v>
+      </c>
       <c r="D12" s="2"/>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-      <c r="H12" s="1"/>
-      <c r="I12" s="1"/>
-      <c r="J12" s="1"/>
-      <c r="K12" s="1"/>
+      <c r="E12" s="1" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="D13" s="2"/>
-      <c r="E13" s="1" t="s">
+      <c r="A13" s="3" t="s">
         <v>67</v>
       </c>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="B14" s="3"/>
-      <c r="C14" s="6"/>
-      <c r="D14" s="8"/>
-      <c r="E14" s="3" t="n">
+      <c r="B13" s="3"/>
+      <c r="C13" s="6"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="3" t="n">
         <v>8</v>
       </c>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="6"/>
-      <c r="I14" s="6"/>
-      <c r="J14" s="3"/>
-      <c r="K14" s="6"/>
-    </row>
-    <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="3"/>
+      <c r="K13" s="6"/>
+    </row>
+    <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
@@ -1904,13 +1890,13 @@
         <v>2</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>69</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>70</v>
       </c>
       <c r="G1" s="1" t="s">
         <v>4</v>
@@ -1918,119 +1904,119 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B2" s="2" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
         <v>73</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>74</v>
       </c>
       <c r="F2" s="1" t="n">
         <v>0.1</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B3" s="2" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C3" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="D3" s="1" t="s">
-        <v>73</v>
-      </c>
       <c r="E3" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F3" s="1" t="n">
         <v>0.1</v>
       </c>
       <c r="G3" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="H3" s="1" t="s">
         <v>78</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B4" s="2" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C4" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>73</v>
-      </c>
       <c r="E4" s="1" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F4" s="1" t="n">
         <v>0.1</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="B5" s="2" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>81</v>
-      </c>
-      <c r="B5" s="2" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>82</v>
       </c>
       <c r="F5" s="1" t="n">
         <v>0.1</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B6" s="2" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="B6" s="2" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="C6" s="1" t="s">
+      <c r="D6" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>85</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>86</v>
       </c>
       <c r="F6" s="1" t="n">
         <v>0.1</v>
@@ -2041,55 +2027,55 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B7" s="2" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="C7" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D7" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>73</v>
-      </c>
       <c r="E7" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="F7" s="1" t="n">
         <v>0.1</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B8" s="2" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
       <c r="C8" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>73</v>
-      </c>
       <c r="E8" s="1" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F8" s="1" t="n">
         <v>0.1</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B9" s="2" t="n">
         <f aca="false">FALSE()</f>
@@ -2099,7 +2085,7 @@
         <v>8</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E9" s="1" t="s">
         <v>24</v>
@@ -2160,66 +2146,66 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="2" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>94</v>
-      </c>
-      <c r="D2" s="2" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="C3" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="2" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="E3" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>98</v>
-      </c>
-      <c r="D3" s="2" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="E3" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>99</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D4" s="2" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>100</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="C4" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="D4" s="2" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>101</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D5" s="2" t="n">
         <f aca="false">FALSE()</f>
@@ -2232,13 +2218,13 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="B6" s="1" t="s">
-        <v>104</v>
-      </c>
       <c r="C6" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="D6" s="2" t="n">
         <f aca="false">FALSE()</f>
@@ -2294,24 +2280,24 @@
         <v>4</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D2" s="2" t="n">
         <f aca="false">FALSE()</f>
         <v>0</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D3" s="2"/>
       <c r="E3" s="1" t="n">
@@ -2320,7 +2306,7 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D4" s="2" t="n">
         <f aca="false">FALSE()</f>
@@ -2332,19 +2318,19 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="D5" s="2" t="n">
+        <f aca="false">FALSE()</f>
+        <v>0</v>
+      </c>
+      <c r="E5" s="1" t="s">
         <v>109</v>
-      </c>
-      <c r="D5" s="2" t="n">
-        <f aca="false">FALSE()</f>
-        <v>0</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D6" s="2" t="n">
         <f aca="false">FALSE()</f>
@@ -2384,7 +2370,7 @@
   <sheetFormatPr defaultColWidth="9.265625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="27.78"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="17.64"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="17.64"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="15.76"/>
   </cols>
   <sheetData>
@@ -2410,28 +2396,28 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>112</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>115</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B5" s="1" t="n">
         <v>40</v>
@@ -2439,7 +2425,7 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B6" s="1" t="n">
         <v>1</v>
@@ -2447,15 +2433,15 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>119</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B8" s="1" t="n">
         <v>0.25</v>
@@ -2463,7 +2449,7 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B9" s="1" t="n">
         <v>0</v>
@@ -2520,23 +2506,32 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="B2" s="1" t="s">
+    </row>
+    <row r="3" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>114</v>
-      </c>
+      <c r="B3" s="0"/>
+      <c r="C3" s="0"/>
+      <c r="D3" s="0"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="0"/>
+      <c r="H3" s="0"/>
+      <c r="I3" s="0"/>
+      <c r="J3" s="0"/>
     </row>
     <row r="4" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>115</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>116</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -2547,17 +2542,15 @@
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
     </row>
-    <row r="5" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B5" s="1" t="n">
         <v>40</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
@@ -2565,7 +2558,7 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B6" s="1" t="n">
         <v>1</v>
@@ -2579,10 +2572,10 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
@@ -2593,7 +2586,7 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B8" s="1" t="n">
         <v>2</v>
@@ -2648,41 +2641,41 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>112</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>115</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B7" s="1" t="n">
         <v>2</v>
@@ -2741,23 +2734,32 @@
     </row>
     <row r="2" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="B2" s="1" t="s">
+    </row>
+    <row r="3" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="1" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="1" t="s">
-        <v>114</v>
-      </c>
+      <c r="B3" s="0"/>
+      <c r="C3" s="0"/>
+      <c r="D3" s="0"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
+      <c r="G3" s="0"/>
+      <c r="H3" s="0"/>
+      <c r="I3" s="0"/>
+      <c r="J3" s="0"/>
     </row>
     <row r="4" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -2768,17 +2770,15 @@
       <c r="I4" s="1"/>
       <c r="J4" s="1"/>
     </row>
-    <row r="5" s="6" customFormat="true" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B5" s="1" t="n">
         <v>0</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
-      <c r="E5" s="1"/>
-      <c r="F5" s="1"/>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
@@ -2786,7 +2786,7 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B6" s="1"/>
       <c r="C6" s="1"/>
@@ -2798,10 +2798,10 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
@@ -2812,7 +2812,7 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B8" s="1" t="n">
         <v>2</v>

</xml_diff>

<commit_message>
PatchManager works. It needs to implement zoom
</commit_message>
<xml_diff>
--- a/configurations/experiment_configs_liver.xlsx
+++ b/configurations/experiment_configs_liver.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="8"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="model_params" sheetId="1" state="visible" r:id="rId3"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="136">
   <si>
     <t xml:space="preserve">var_name</t>
   </si>
@@ -387,6 +387,9 @@
   </si>
   <si>
     <t xml:space="preserve">expand_by</t>
+  </si>
+  <si>
+    <t xml:space="preserve">src_dest_labels</t>
   </si>
   <si>
     <t xml:space="preserve">lbd</t>
@@ -684,7 +687,7 @@
   <dimension ref="A1:I1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A12" activeCellId="1" sqref="A9:B10 A12"/>
+      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1040,8 +1043,8 @@
   </sheetPr>
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A9:B10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.57421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1097,7 +1100,7 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B6" s="1" t="n">
         <v>1</v>
@@ -1121,21 +1124,25 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+        <v>128</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1156,10 +1163,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A9:B10"/>
+      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.16015625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1225,10 +1232,10 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1236,12 +1243,12 @@
         <v>114</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B9" s="1" t="n">
         <v>2</v>
@@ -1249,18 +1256,23 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="B10" s="0" t="n">
+        <v>123</v>
+      </c>
+      <c r="B10" s="1" t="n">
         <v>128</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="B11" s="0" t="n">
+        <v>124</v>
+      </c>
+      <c r="B11" s="1" t="n">
         <v>96</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>118</v>
       </c>
     </row>
   </sheetData>
@@ -1279,10 +1291,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9:B10"/>
+      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.2578125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1358,7 +1370,7 @@
         <v>114</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
@@ -1369,7 +1381,7 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B8" s="1" t="n">
         <v>2</v>
@@ -1377,18 +1389,23 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="B9" s="0" t="n">
+        <v>123</v>
+      </c>
+      <c r="B9" s="1" t="n">
         <v>128</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="B10" s="0" t="n">
+        <v>124</v>
+      </c>
+      <c r="B10" s="1" t="n">
         <v>96</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>118</v>
       </c>
     </row>
   </sheetData>
@@ -1410,7 +1427,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="1" sqref="A9:B10 A8"/>
+      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.16015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1470,7 +1487,7 @@
         <v>114</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C5" s="1"/>
       <c r="D5" s="1"/>
@@ -1479,17 +1496,17 @@
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B7" s="1" t="n">
         <v>1</v>
@@ -1498,6 +1515,9 @@
       <c r="F7" s="1"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>118</v>
+      </c>
       <c r="B8" s="4"/>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
@@ -1521,7 +1541,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="1" sqref="A9:B10 B3"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.16015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1551,7 +1571,7 @@
         <v>107</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="C2" s="1"/>
     </row>
@@ -1608,7 +1628,7 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="B9" s="1" t="n">
         <v>0</v>
@@ -1634,7 +1654,7 @@
   <dimension ref="A1:K1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E13" activeCellId="1" sqref="A9:B10 E13"/>
+      <selection pane="topLeft" activeCell="B17" activeCellId="0" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1838,7 +1858,7 @@
       <c r="C13" s="6"/>
       <c r="D13" s="8"/>
       <c r="E13" s="3" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
@@ -1870,7 +1890,7 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G7" activeCellId="1" sqref="A9:B10 G7"/>
+      <selection pane="topLeft" activeCell="G7" activeCellId="0" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.265625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2120,7 +2140,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E7" activeCellId="1" sqref="A9:B10 E7"/>
+      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2256,7 +2276,7 @@
   <dimension ref="A1:F1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A7" activeCellId="1" sqref="A9:B10 A7"/>
+      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2364,10 +2384,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A9:B10"/>
+      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.265625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2456,6 +2476,11 @@
       </c>
       <c r="B9" s="1" t="n">
         <v>0</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>118</v>
       </c>
     </row>
   </sheetData>
@@ -2474,10 +2499,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J8"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B8" activeCellId="1" sqref="A9:B10 B8"/>
+      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.2578125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2578,7 +2603,7 @@
         <v>114</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
@@ -2589,10 +2614,15 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B8" s="1" t="n">
         <v>2</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="1" t="s">
+        <v>118</v>
       </c>
     </row>
   </sheetData>
@@ -2614,7 +2644,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A7" activeCellId="1" sqref="A9:B10 A7"/>
+      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23828125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2673,18 +2703,22 @@
         <v>114</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B7" s="1" t="n">
         <v>2</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="1" t="s">
+        <v>118</v>
+      </c>
+    </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -2702,10 +2736,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9:B10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.2578125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2762,7 +2796,7 @@
         <v>110</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -2804,7 +2838,7 @@
         <v>114</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C7" s="1"/>
       <c r="D7" s="1"/>
@@ -2815,7 +2849,7 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B8" s="1" t="n">
         <v>2</v>
@@ -2823,18 +2857,23 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>122</v>
-      </c>
-      <c r="B9" s="0" t="n">
+        <v>123</v>
+      </c>
+      <c r="B9" s="1" t="n">
         <v>128</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>123</v>
-      </c>
-      <c r="B10" s="0" t="n">
+        <v>124</v>
+      </c>
+      <c r="B10" s="1" t="n">
         <v>96</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>118</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
multiple bug fixes. New pipelines introduced
</commit_message>
<xml_diff>
--- a/configurations/experiment_configs_liver.xlsx
+++ b/configurations/experiment_configs_liver.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="9"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="model_params" sheetId="1" state="visible" r:id="rId3"/>
@@ -1050,8 +1050,8 @@
   </sheetPr>
   <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.2578125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1810,7 +1810,7 @@
   </sheetPr>
   <dimension ref="A1:K1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
     </sheetView>
   </sheetViews>
@@ -2018,7 +2018,7 @@
       <c r="C13" s="6"/>
       <c r="D13" s="8"/>
       <c r="E13" s="3" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
@@ -2032,7 +2032,7 @@
         <v>64</v>
       </c>
       <c r="E14" s="1" t="n">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="G14" s="1" t="s">
         <v>65</v>

</xml_diff>

<commit_message>
Loss function breaks for 2 class outputs
</commit_message>
<xml_diff>
--- a/configurations/experiment_configs_liver.xlsx
+++ b/configurations/experiment_configs_liver.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="8"/>
   </bookViews>
   <sheets>
     <sheet name="model_params" sheetId="1" state="visible" r:id="rId3"/>
@@ -691,7 +691,7 @@
   <dimension ref="A1:J1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
+      <selection pane="topLeft" activeCell="E2" activeCellId="1" sqref="C:C E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1051,7 +1051,7 @@
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
+      <selection pane="topLeft" activeCell="B9" activeCellId="1" sqref="C:C B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.2578125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1209,7 +1209,7 @@
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
+      <selection pane="topLeft" activeCell="A9" activeCellId="1" sqref="C:C A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.57421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1323,7 +1323,7 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
+      <selection pane="topLeft" activeCell="A12" activeCellId="1" sqref="C:C A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.16015625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1451,7 +1451,7 @@
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A11" activeCellId="0" sqref="A11"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="1" sqref="C:C B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.2578125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1584,7 +1584,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+      <selection pane="topLeft" activeCell="A8" activeCellId="1" sqref="C:C A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.16015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1698,7 +1698,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="1" sqref="C:C B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.16015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1810,8 +1810,8 @@
   </sheetPr>
   <dimension ref="A1:K1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C35" activeCellId="0" sqref="C35"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C35" activeCellId="0" sqref="C:C"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2065,7 +2065,7 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G7" activeCellId="0" sqref="G7"/>
+      <selection pane="topLeft" activeCell="G7" activeCellId="1" sqref="C:C G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.265625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2315,7 +2315,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
+      <selection pane="topLeft" activeCell="E7" activeCellId="1" sqref="C:C E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2451,7 +2451,7 @@
   <dimension ref="A1:F1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
+      <selection pane="topLeft" activeCell="A7" activeCellId="1" sqref="C:C A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2562,7 +2562,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
+      <selection pane="topLeft" activeCell="A10" activeCellId="1" sqref="C:C A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.265625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2677,7 +2677,7 @@
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="1" sqref="C:C B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.2578125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2826,7 +2826,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
+      <selection pane="topLeft" activeCell="A8" activeCellId="1" sqref="C:C A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23828125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2920,13 +2920,14 @@
   </sheetPr>
   <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C:C"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.2578125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="23.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="29.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="28.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="25.57"/>
   </cols>

</xml_diff>

<commit_message>
many changes done. Plans are now saved in database. Now reducing inference memory footprint, using yiekd
</commit_message>
<xml_diff>
--- a/configurations/experiment_configs_liver.xlsx
+++ b/configurations/experiment_configs_liver.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="8"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="model_params" sheetId="1" state="visible" r:id="rId3"/>
@@ -22,7 +22,7 @@
     <sheet name="plan6" sheetId="12" state="visible" r:id="rId14"/>
     <sheet name="plan7" sheetId="13" state="visible" r:id="rId15"/>
     <sheet name="plan8" sheetId="14" state="visible" r:id="rId16"/>
-    <sheet name="plantmp" sheetId="15" state="visible" r:id="rId17"/>
+    <sheet name="plan10" sheetId="15" state="visible" r:id="rId17"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="135">
   <si>
     <t xml:space="preserve">var_name</t>
   </si>
@@ -408,18 +408,18 @@
     <t xml:space="preserve">samples_per_file</t>
   </si>
   <si>
+    <t xml:space="preserve">patch_dim0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">patch_dim1</t>
+  </si>
+  <si>
     <t xml:space="preserve">source</t>
   </si>
   <si>
     <t xml:space="preserve">0.8,0.8,1.5</t>
   </si>
   <si>
-    <t xml:space="preserve">patch_dim0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">patch_dim1</t>
-  </si>
-  <si>
     <t xml:space="preserve">source_plan</t>
   </si>
   <si>
@@ -439,12 +439,6 @@
   </si>
   <si>
     <t xml:space="preserve">plan7</t>
-  </si>
-  <si>
-    <t xml:space="preserve">drli_short</t>
-  </si>
-  <si>
-    <t xml:space="preserve">expand_by_patch</t>
   </si>
 </sst>
 </file>
@@ -691,7 +685,7 @@
   <dimension ref="A1:J1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E2" activeCellId="1" sqref="C:C E2"/>
+      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1051,7 +1045,7 @@
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B9" activeCellId="1" sqref="C:C B9"/>
+      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.2578125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1112,7 +1106,7 @@
         <v>113</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -1171,7 +1165,7 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B9" s="1" t="n">
         <v>224</v>
@@ -1179,7 +1173,7 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B10" s="1" t="n">
         <v>96</v>
@@ -1209,7 +1203,7 @@
   <dimension ref="A1:F14"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A9" activeCellId="1" sqref="C:C A9"/>
+      <selection pane="topLeft" activeCell="A9" activeCellId="0" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.57421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1323,7 +1317,7 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A12" activeCellId="1" sqref="C:C A12"/>
+      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.16015625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1413,7 +1407,7 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B10" s="1" t="n">
         <v>128</v>
@@ -1421,7 +1415,7 @@
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B11" s="1" t="n">
         <v>96</v>
@@ -1451,7 +1445,7 @@
   <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="1" sqref="C:C B1"/>
+      <selection pane="topLeft" activeCell="B1" activeCellId="0" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.2578125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1546,7 +1540,7 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B9" s="1" t="n">
         <v>128</v>
@@ -1554,7 +1548,7 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B10" s="1" t="n">
         <v>96</v>
@@ -1584,7 +1578,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="1" sqref="C:C A8"/>
+      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.16015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1695,10 +1689,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="1" sqref="C:C B3"/>
+      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.16015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1728,15 +1722,22 @@
         <v>110</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>135</v>
+        <v>111</v>
       </c>
       <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
         <v>112</v>
       </c>
+      <c r="B3" s="1"/>
       <c r="C3" s="1"/>
+      <c r="D3" s="1"/>
+      <c r="E3" s="1"/>
+      <c r="F3" s="1"/>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
@@ -1746,15 +1747,21 @@
         <v>114</v>
       </c>
       <c r="C4" s="1"/>
+      <c r="D4" s="1"/>
+      <c r="E4" s="1"/>
+      <c r="F4" s="1"/>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>115</v>
+        <v>120</v>
       </c>
       <c r="B5" s="1" t="n">
         <v>40</v>
       </c>
       <c r="C5" s="1"/>
+      <c r="D5" s="1"/>
+      <c r="E5" s="1"/>
+      <c r="F5" s="1"/>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
@@ -1764,33 +1771,59 @@
         <v>1</v>
       </c>
       <c r="C6" s="1"/>
+      <c r="D6" s="1"/>
+      <c r="E6" s="1"/>
+      <c r="F6" s="1"/>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
         <v>117</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>118</v>
+        <v>122</v>
       </c>
       <c r="C7" s="1"/>
+      <c r="D7" s="1"/>
+      <c r="E7" s="1"/>
+      <c r="F7" s="1"/>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
-        <v>119</v>
+        <v>123</v>
       </c>
       <c r="B8" s="1" t="n">
-        <v>0.25</v>
-      </c>
-      <c r="C8" s="1"/>
+        <v>1</v>
+      </c>
+      <c r="E8" s="1"/>
+      <c r="F8" s="1"/>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="B9" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="C9" s="1"/>
+        <v>121</v>
+      </c>
+      <c r="B9" s="1"/>
+      <c r="E9" s="1"/>
+      <c r="F9" s="1"/>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B10" s="1" t="n">
+        <v>128</v>
+      </c>
+      <c r="E10" s="1"/>
+      <c r="F10" s="1"/>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B11" s="1" t="n">
+        <v>96</v>
+      </c>
+      <c r="E11" s="1"/>
+      <c r="F11" s="1"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -1810,8 +1843,8 @@
   </sheetPr>
   <dimension ref="A1:K1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C35" activeCellId="0" sqref="C:C"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1852,7 +1885,7 @@
         <v>0</v>
       </c>
       <c r="E2" s="6" t="n">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2018,7 +2051,7 @@
       <c r="C13" s="6"/>
       <c r="D13" s="8"/>
       <c r="E13" s="3" t="n">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
@@ -2032,7 +2065,7 @@
         <v>64</v>
       </c>
       <c r="E14" s="1" t="n">
-        <v>4</v>
+        <v>10</v>
       </c>
       <c r="G14" s="1" t="s">
         <v>65</v>
@@ -2065,7 +2098,7 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G7" activeCellId="1" sqref="C:C G7"/>
+      <selection pane="topLeft" activeCell="G7" activeCellId="0" sqref="G7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.265625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2315,7 +2348,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E7" activeCellId="1" sqref="C:C E7"/>
+      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2451,7 +2484,7 @@
   <dimension ref="A1:F1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A7" activeCellId="1" sqref="C:C A7"/>
+      <selection pane="topLeft" activeCell="A7" activeCellId="0" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.265625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2562,7 +2595,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A10" activeCellId="1" sqref="C:C A10"/>
+      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.265625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2674,10 +2707,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B1" activeCellId="1" sqref="C:C B1"/>
+      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.2578125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2805,6 +2838,22 @@
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
         <v>121</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="B10" s="1" t="n">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="B11" s="1" t="n">
+        <v>96</v>
       </c>
     </row>
   </sheetData>
@@ -2826,7 +2875,7 @@
   <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A8" activeCellId="1" sqref="C:C A8"/>
+      <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23828125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2885,7 +2934,7 @@
         <v>117</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2920,14 +2969,14 @@
   </sheetPr>
   <dimension ref="A1:J11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C:C"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A10" activeCellId="0" sqref="A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.2578125" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="23.59"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="29.29"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="29.3"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="28.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="25.57"/>
   </cols>
@@ -2987,7 +3036,7 @@
         <v>113</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
@@ -3014,7 +3063,6 @@
       <c r="A6" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="B6" s="1"/>
       <c r="C6" s="1"/>
       <c r="D6" s="1"/>
       <c r="G6" s="1"/>
@@ -3046,7 +3094,7 @@
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B9" s="1" t="n">
         <v>128</v>
@@ -3054,7 +3102,7 @@
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B10" s="1" t="n">
         <v>96</v>

</xml_diff>

<commit_message>
Multiple fixes. imported labelmap classes work now
</commit_message>
<xml_diff>
--- a/configurations/experiment_configs_liver.xlsx
+++ b/configurations/experiment_configs_liver.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="528" uniqueCount="172">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="529" uniqueCount="173">
   <si>
     <t xml:space="preserve">var_name</t>
   </si>
@@ -527,6 +527,9 @@
   </si>
   <si>
     <t xml:space="preserve">use_fg_indices</t>
+  </si>
+  <si>
+    <t xml:space="preserve">imported_folder</t>
   </si>
   <si>
     <t xml:space="preserve">plan1</t>
@@ -1851,17 +1854,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Y11"/>
+  <dimension ref="A1:Z11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="N1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="S7" activeCellId="0" sqref="S7"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="M1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="Y12" activeCellId="0" sqref="Y12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.7578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="17.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="0" width="8.59"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="20" style="3" width="8.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="13.97"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="3" width="13.97"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="3" width="13.97"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="22" style="3" width="8.59"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1923,27 +1928,30 @@
         <v>163</v>
       </c>
       <c r="T1" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="U1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="U1" s="1" t="s">
+      <c r="V1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="V1" s="1" t="s">
+      <c r="W1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="W1" s="1" t="s">
+      <c r="X1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="X1" s="1" t="s">
+      <c r="Y1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="Y1" s="1" t="s">
+      <c r="Z1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="2" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>129</v>
@@ -1969,14 +1977,15 @@
       <c r="R2" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="S2" s="4" t="b">
+      <c r="S2" s="4" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="T2" s="2"/>
+      <c r="U2" s="2"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>129</v>
@@ -2002,13 +2011,14 @@
       <c r="R3" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="S3" s="4" t="b">
+      <c r="S3" s="4" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>129</v>
@@ -2022,10 +2032,11 @@
       <c r="R4" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="S4" s="4" t="b">
+      <c r="S4" s="4" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="T4" s="2"/>
+      <c r="U4" s="2"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
@@ -2052,14 +2063,15 @@
       <c r="R5" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="S5" s="4" t="b">
+      <c r="S5" s="4" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="T5" s="2"/>
+      <c r="U5" s="2"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>129</v>
@@ -2082,14 +2094,15 @@
       <c r="R6" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="S6" s="4" t="b">
+      <c r="S6" s="4" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="T6" s="2"/>
+      <c r="U6" s="2"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>129</v>
@@ -2112,14 +2125,15 @@
       <c r="R7" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="S7" s="4" t="b">
+      <c r="S7" s="4" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="T7" s="2"/>
+      <c r="U7" s="2"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>129</v>
@@ -2145,10 +2159,11 @@
       <c r="R8" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="S8" s="4" t="b">
+      <c r="S8" s="4" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="T8" s="2"/>
+      <c r="U8" s="2"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
@@ -2175,14 +2190,15 @@
       <c r="R9" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="S9" s="4" t="b">
+      <c r="S9" s="4" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="T9" s="2"/>
+      <c r="U9" s="2"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>170</v>
+        <v>171</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>129</v>
@@ -2196,13 +2212,14 @@
       <c r="Q10" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="S10" s="4" t="b">
+      <c r="S10" s="4" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
-        <v>171</v>
+        <v>172</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>129</v>
@@ -2228,7 +2245,8 @@
       <c r="R11" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="S11" s="4" t="b">
+      <c r="S11" s="4" t="n">
+        <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fixes many. about to change db critical funcs
</commit_message>
<xml_diff>
--- a/configurations/experiment_configs_liver.xlsx
+++ b/configurations/experiment_configs_liver.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="529" uniqueCount="173">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="519" uniqueCount="165">
   <si>
     <t xml:space="preserve">var_name</t>
   </si>
@@ -530,30 +530,6 @@
   </si>
   <si>
     <t xml:space="preserve">imported_folder</t>
-  </si>
-  <si>
-    <t xml:space="preserve">plan1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">plan2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">plan3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">plan9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">plan5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">plan6</t>
-  </si>
-  <si>
-    <t xml:space="preserve">plan8</t>
-  </si>
-  <si>
-    <t xml:space="preserve">plan11</t>
   </si>
 </sst>
 </file>
@@ -860,7 +836,7 @@
   <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="A2:A11 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1188,7 +1164,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="A2:A11 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1303,7 +1279,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="A2:A11 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1410,7 +1386,7 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="A2:A11 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1533,7 +1509,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="A2:A11 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1648,7 +1624,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="A2:A11 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1739,7 +1715,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="A2:A11 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1856,15 +1832,14 @@
   </sheetPr>
   <dimension ref="A1:Z11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="M1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="Y12" activeCellId="0" sqref="Y12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2:A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.7578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="17.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="18" style="0" width="13.97"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="19" style="3" width="13.97"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="18" style="3" width="13.97"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="3" width="13.97"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="22" style="3" width="8.59"/>
   </cols>
@@ -1950,8 +1925,8 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
-        <v>165</v>
+      <c r="A2" s="2" t="n">
+        <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>129</v>
@@ -1984,8 +1959,8 @@
       <c r="U2" s="2"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2" t="s">
-        <v>166</v>
+      <c r="A3" s="2" t="n">
+        <v>2</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>129</v>
@@ -2017,8 +1992,8 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="s">
-        <v>167</v>
+      <c r="A4" s="2" t="n">
+        <v>3</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>129</v>
@@ -2039,8 +2014,8 @@
       <c r="U4" s="2"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2" t="s">
-        <v>152</v>
+      <c r="A5" s="2" t="n">
+        <v>4</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>129</v>
@@ -2070,8 +2045,8 @@
       <c r="U5" s="2"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2" t="s">
-        <v>168</v>
+      <c r="A6" s="2" t="n">
+        <v>9</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>129</v>
@@ -2101,8 +2076,8 @@
       <c r="U6" s="2"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="2" t="s">
-        <v>169</v>
+      <c r="A7" s="2" t="n">
+        <v>5</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>129</v>
@@ -2132,8 +2107,8 @@
       <c r="U7" s="2"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="2" t="s">
-        <v>170</v>
+      <c r="A8" s="2" t="n">
+        <v>6</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>129</v>
@@ -2166,8 +2141,8 @@
       <c r="U8" s="2"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="2" t="s">
-        <v>158</v>
+      <c r="A9" s="2" t="n">
+        <v>7</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>129</v>
@@ -2197,8 +2172,8 @@
       <c r="U9" s="2"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="2" t="s">
-        <v>171</v>
+      <c r="A10" s="2" t="n">
+        <v>8</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>129</v>
@@ -2218,8 +2193,8 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="2" t="s">
-        <v>172</v>
+      <c r="A11" s="2" t="n">
+        <v>11</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>129</v>
@@ -2269,7 +2244,7 @@
   <dimension ref="A1:K28"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
+      <selection pane="topLeft" activeCell="E15" activeCellId="1" sqref="A2:A11 E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2475,7 +2450,7 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="A2:A11 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2712,7 +2687,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="A2:A11 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2835,7 +2810,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="A2:A11 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2928,7 +2903,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
+      <selection pane="topLeft" activeCell="F1" activeCellId="1" sqref="A2:A11 F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3038,7 +3013,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="A2:A11 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3156,7 +3131,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="A2:A11 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3247,7 +3222,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="A2:A11 A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
moved away from table master_plans, hash codes for folder names
</commit_message>
<xml_diff>
--- a/configurations/experiment_configs_liver.xlsx
+++ b/configurations/experiment_configs_liver.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="519" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="516" uniqueCount="165">
   <si>
     <t xml:space="preserve">var_name</t>
   </si>
@@ -836,7 +836,7 @@
   <dimension ref="A1:J17"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="A2:A11 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1164,7 +1164,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="A2:A11 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1279,7 +1279,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="A2:A11 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1386,7 +1386,7 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="A2:A11 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1509,7 +1509,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="A2:A11 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1624,7 +1624,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="A2:A11 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1715,7 +1715,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="A2:A11 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1830,18 +1830,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:Z11"/>
+  <dimension ref="A1:Y11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2:A11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="C1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.7578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="2" width="17.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="19" min="18" style="3" width="13.97"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="21" style="3" width="13.97"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="25" min="22" style="3" width="8.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="18" min="17" style="3" width="13.97"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="20" min="20" style="3" width="13.97"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="24" min="21" style="3" width="8.59"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="16384" min="16384" style="0" width="10.16"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1855,72 +1855,69 @@
         <v>140</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>130</v>
+        <v>136</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>136</v>
+        <v>144</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>138</v>
+        <v>160</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="M1" s="1" t="s">
-        <v>162</v>
+        <v>141</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>141</v>
+        <v>153</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>153</v>
+        <v>143</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>143</v>
+        <v>151</v>
       </c>
       <c r="Q1" s="1" t="s">
-        <v>151</v>
+        <v>131</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>131</v>
+        <v>163</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="T1" s="1" t="s">
-        <v>164</v>
+        <v>4</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="V1" s="1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="W1" s="1" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="X1" s="1" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="Y1" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="Z1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
@@ -1931,32 +1928,29 @@
       <c r="B2" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>34</v>
+      <c r="C2" s="2" t="n">
+        <v>40</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>134</v>
-      </c>
-      <c r="E2" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="J2" s="2" t="s">
+      <c r="I2" s="2" t="s">
         <v>139</v>
       </c>
+      <c r="J2" s="2"/>
       <c r="K2" s="2"/>
       <c r="L2" s="2"/>
-      <c r="M2" s="2"/>
-      <c r="R2" s="2" t="s">
+      <c r="Q2" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="S2" s="4" t="n">
+      <c r="R2" s="4" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="U2" s="2"/>
+      <c r="T2" s="2"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="n">
@@ -1968,25 +1962,25 @@
       <c r="C3" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>24</v>
       </c>
+      <c r="F3" s="2" t="s">
+        <v>142</v>
+      </c>
       <c r="G3" s="2" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="I3" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="P3" s="2" t="s">
+      <c r="O3" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="R3" s="2" t="s">
+      <c r="Q3" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="S3" s="4" t="n">
+      <c r="R3" s="4" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -1998,20 +1992,20 @@
       <c r="B4" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="G4" s="2" t="s">
+      <c r="F4" s="2" t="s">
         <v>148</v>
       </c>
-      <c r="P4" s="2" t="s">
+      <c r="O4" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="R4" s="2" t="s">
+      <c r="Q4" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="S4" s="4" t="n">
+      <c r="R4" s="4" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="U4" s="2"/>
+      <c r="T4" s="2"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="n">
@@ -2023,26 +2017,26 @@
       <c r="C5" s="2" t="s">
         <v>61</v>
       </c>
+      <c r="F5" s="2" t="s">
+        <v>142</v>
+      </c>
       <c r="G5" s="2" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="I5" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="P5" s="2" t="s">
+      <c r="O5" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="R5" s="2" t="s">
+      <c r="Q5" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="S5" s="4" t="n">
+      <c r="R5" s="4" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="U5" s="2"/>
+      <c r="T5" s="2"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="n">
@@ -2054,26 +2048,26 @@
       <c r="C6" s="2" t="s">
         <v>34</v>
       </c>
+      <c r="F6" s="2" t="s">
+        <v>142</v>
+      </c>
       <c r="G6" s="2" t="s">
-        <v>142</v>
+        <v>150</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="I6" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="P6" s="2" t="s">
+      <c r="O6" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="R6" s="2" t="s">
+      <c r="Q6" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="S6" s="4" t="n">
+      <c r="R6" s="4" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="U6" s="2"/>
+      <c r="T6" s="2"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="n">
@@ -2082,29 +2076,29 @@
       <c r="B7" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="G7" s="2" t="s">
+      <c r="F7" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="J7" s="2" t="s">
+      <c r="I7" s="2" t="s">
         <v>139</v>
       </c>
+      <c r="J7" s="2"/>
       <c r="K7" s="2"/>
       <c r="L7" s="2"/>
-      <c r="M7" s="2"/>
+      <c r="O7" s="2" t="s">
+        <v>24</v>
+      </c>
       <c r="P7" s="2" t="s">
-        <v>24</v>
+        <v>152</v>
       </c>
       <c r="Q7" s="2" t="s">
-        <v>152</v>
-      </c>
-      <c r="R7" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="S7" s="4" t="n">
+      <c r="R7" s="4" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="U7" s="2"/>
+      <c r="T7" s="2"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="n">
@@ -2116,29 +2110,29 @@
       <c r="C8" s="2" t="s">
         <v>134</v>
       </c>
+      <c r="F8" s="2" t="s">
+        <v>155</v>
+      </c>
       <c r="G8" s="2" t="s">
-        <v>155</v>
+        <v>145</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="I8" s="2" t="s">
         <v>147</v>
       </c>
+      <c r="N8" s="2" t="s">
+        <v>154</v>
+      </c>
       <c r="O8" s="2" t="s">
-        <v>154</v>
-      </c>
-      <c r="P8" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="R8" s="2" t="s">
+      <c r="Q8" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="S8" s="4" t="n">
+      <c r="R8" s="4" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="U8" s="2"/>
+      <c r="T8" s="2"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="n">
@@ -2150,26 +2144,26 @@
       <c r="C9" s="2" t="s">
         <v>156</v>
       </c>
+      <c r="F9" s="2" t="s">
+        <v>142</v>
+      </c>
       <c r="G9" s="2" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="I9" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="P9" s="2" t="s">
+      <c r="O9" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="R9" s="2" t="s">
+      <c r="Q9" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="S9" s="4" t="n">
+      <c r="R9" s="4" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
-      <c r="U9" s="2"/>
+      <c r="T9" s="2"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="n">
@@ -2178,16 +2172,16 @@
       <c r="B10" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="G10" s="2" t="s">
+      <c r="F10" s="2" t="s">
         <v>157</v>
       </c>
+      <c r="O10" s="2" t="s">
+        <v>24</v>
+      </c>
       <c r="P10" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q10" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="S10" s="4" t="n">
+      <c r="R10" s="4" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -2202,25 +2196,25 @@
       <c r="C11" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="E11" s="2" t="s">
+      <c r="D11" s="2" t="s">
         <v>24</v>
       </c>
+      <c r="F11" s="2" t="s">
+        <v>142</v>
+      </c>
       <c r="G11" s="2" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>145</v>
-      </c>
-      <c r="I11" s="2" t="s">
         <v>147</v>
       </c>
-      <c r="P11" s="2" t="s">
+      <c r="O11" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="R11" s="2" t="s">
+      <c r="Q11" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="S11" s="4" t="n">
+      <c r="R11" s="4" t="n">
         <f aca="false">TRUE()</f>
         <v>1</v>
       </c>
@@ -2244,7 +2238,7 @@
   <dimension ref="A1:K28"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E15" activeCellId="1" sqref="A2:A11 E15"/>
+      <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2450,7 +2444,7 @@
   <dimension ref="A1:H9"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="A2:A11 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2687,7 +2681,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="A2:A11 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2810,7 +2804,7 @@
   <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="A2:A11 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2903,7 +2897,7 @@
   <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F1" activeCellId="1" sqref="A2:A11 F1"/>
+      <selection pane="topLeft" activeCell="F1" activeCellId="0" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3013,7 +3007,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="A2:A11 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3131,7 +3125,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="A2:A11 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3222,7 +3216,7 @@
   <dimension ref="A1:F11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="1" sqref="A2:A11 A1"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
changes in installation default
</commit_message>
<xml_diff>
--- a/configurations/experiment_configs_liver.xlsx
+++ b/configurations/experiment_configs_liver.xlsx
@@ -111,7 +111,7 @@
     <t xml:space="preserve">lr</t>
   </si>
   <si>
-    <t xml:space="preserve">[1e-2,5e-4]</t>
+    <t xml:space="preserve">[1e-4,5e-2]</t>
   </si>
   <si>
     <t xml:space="preserve">qloguniform</t>
@@ -637,23 +637,6 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF000000"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
 </styleSheet>
 </file>
 
@@ -839,11 +822,16 @@
   </sheetPr>
   <dimension ref="A1:J17"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B6" activeCellId="0" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="47.91"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="3" style="0" width="20.09"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1167,13 +1155,15 @@
   </sheetPr>
   <dimension ref="A1:K28"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D6" activeCellId="0" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="19.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="1" style="0" width="14.21"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="3" width="19.15"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="6" style="0" width="21.56"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1226,6 +1216,9 @@
       <c r="A3" s="2" t="s">
         <v>58</v>
       </c>
+      <c r="D3" s="0" t="n">
+        <v>1</v>
+      </c>
       <c r="E3" s="2" t="s">
         <v>24</v>
       </c>
@@ -1244,6 +1237,9 @@
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
         <v>62</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>1</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>63</v>
@@ -1376,11 +1372,14 @@
   </sheetPr>
   <dimension ref="A1:H9"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="1" style="0" width="18.38"/>
+  </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
@@ -1613,7 +1612,7 @@
   </sheetPr>
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -1736,7 +1735,7 @@
   </sheetPr>
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
@@ -1829,7 +1828,7 @@
   </sheetPr>
   <dimension ref="A1:Y11"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A8" activeCellId="0" sqref="A8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Fixed bug in labelboundeddatagenerator
</commit_message>
<xml_diff>
--- a/configurations/experiment_configs_liver.xlsx
+++ b/configurations/experiment_configs_liver.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="297" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="163">
   <si>
     <t xml:space="preserve">var_name</t>
   </si>
@@ -210,9 +210,6 @@
     <t xml:space="preserve">src_dim1</t>
   </si>
   <si>
-    <t xml:space="preserve">[192,192,128]</t>
-  </si>
-  <si>
     <t xml:space="preserve">[192,192,96]</t>
   </si>
   <si>
@@ -280,9 +277,6 @@
   </si>
   <si>
     <t xml:space="preserve">This is the plan used to create validation dataset regardless of which plan training dataset is from. This ensures dice scores of validation ds are comparable across plans</t>
-  </si>
-  <si>
-    <t xml:space="preserve">jk</t>
   </si>
   <si>
     <t xml:space="preserve">tune_p</t>
@@ -1159,7 +1153,7 @@
   <dimension ref="A1:K1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D19" activeCellId="0" sqref="D19"/>
+      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1222,44 +1216,47 @@
       <c r="A3" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="B3" s="1" t="n">
+      <c r="B3" s="3"/>
+      <c r="D3" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E3" s="3" t="n">
         <v>192</v>
       </c>
-      <c r="E3" s="3"/>
       <c r="G3" s="3"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="B4" s="1" t="n">
+      <c r="D4" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E4" s="3" t="n">
         <v>128</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="F4" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="G4" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="H4" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="I4" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="J4" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="J4" s="3" t="s">
+      <c r="K4" s="3" t="s">
         <v>66</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="D5" s="3" t="n">
         <v>0</v>
@@ -1270,10 +1267,10 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>69</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>70</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>12</v>
@@ -1282,15 +1279,15 @@
         <v>0</v>
       </c>
       <c r="E6" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="I6" s="3" t="s">
         <v>71</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>20</v>
@@ -1307,32 +1304,32 @@
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="D8" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" s="3" t="s">
         <v>75</v>
-      </c>
-      <c r="D8" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="E9" s="3" t="s">
         <v>77</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>79</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>80</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>35</v>
@@ -1340,12 +1337,12 @@
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="E12" s="3" t="n">
         <v>11</v>
@@ -1353,19 +1350,17 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="E13" s="3" t="n">
         <v>11</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="3" t="s">
-        <v>85</v>
-      </c>
+      <c r="B27" s="3"/>
     </row>
     <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1408,13 +1403,13 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>1</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>4</v>
@@ -1425,114 +1420,114 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B2" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>88</v>
       </c>
-      <c r="B2" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="C2" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>89</v>
-      </c>
-      <c r="D2" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>91</v>
       </c>
       <c r="F2" s="3" t="n">
         <v>0.1</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B3" s="3" t="n">
         <v>1</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F3" s="3" t="n">
         <v>0.1</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B4" s="3" t="n">
         <v>1</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="F4" s="3" t="n">
         <v>0.1</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B5" s="3" t="n">
         <v>0</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F5" s="3" t="n">
         <v>0.1</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B6" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>101</v>
-      </c>
-      <c r="B6" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>102</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>103</v>
       </c>
       <c r="F6" s="3" t="n">
         <v>0.1</v>
@@ -1543,53 +1538,53 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="B7" s="3" t="n">
         <v>0</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="F7" s="3" t="n">
         <v>0.1</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B8" s="3" t="n">
         <v>1</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="F8" s="3" t="n">
         <v>0.1</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="B9" s="3" t="n">
         <v>0</v>
@@ -1598,7 +1593,7 @@
         <v>12</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>20</v>
@@ -1655,32 +1650,32 @@
         <v>4</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="D2" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>110</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="D2" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="C3" s="3" t="s">
         <v>113</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>115</v>
       </c>
       <c r="D3" s="3" t="n">
         <v>0</v>
@@ -1689,29 +1684,29 @@
         <v>35</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D4" s="3" t="n">
         <v>0</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="D5" s="3" t="n">
         <v>0</v>
@@ -1722,19 +1717,19 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="D6" s="3" t="n">
         <v>0</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
   </sheetData>
@@ -1778,12 +1773,12 @@
         <v>4</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="D2" s="3" t="n">
         <v>0</v>
@@ -1791,7 +1786,7 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>21</v>
@@ -1799,7 +1794,7 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="D4" s="3" t="n">
         <v>0</v>
@@ -1810,18 +1805,18 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="D5" s="3" t="n">
         <v>0</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D6" s="3" t="n">
         <v>0</v>
@@ -1862,61 +1857,61 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>145</v>
-      </c>
-      <c r="R1" s="2" t="s">
-        <v>146</v>
-      </c>
-      <c r="S1" s="2" t="s">
-        <v>147</v>
       </c>
       <c r="T1" s="2" t="s">
         <v>4</v>
@@ -1942,28 +1937,28 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>21</v>
       </c>
       <c r="F2" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="H2" s="3" t="s">
         <v>150</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>152</v>
       </c>
       <c r="O2" s="3" t="s">
         <v>50</v>
       </c>
       <c r="Q2" s="3" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="R2" s="4" t="n">
         <f aca="false">TRUE()</f>
@@ -1975,16 +1970,16 @@
         <v>3</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="O3" s="3" t="s">
         <v>50</v>
       </c>
       <c r="Q3" s="3" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="R3" s="4" t="n">
         <f aca="false">TRUE()</f>
@@ -1997,25 +1992,25 @@
         <v>4</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>78</v>
-      </c>
-      <c r="F4" s="3" t="s">
+      <c r="G4" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="H4" s="3" t="s">
         <v>150</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>152</v>
       </c>
       <c r="O4" s="3" t="s">
         <v>50</v>
       </c>
       <c r="Q4" s="3" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="R4" s="4" t="n">
         <f aca="false">TRUE()</f>
@@ -2028,13 +2023,13 @@
         <v>5</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="J5" s="3"/>
       <c r="K5" s="3"/>
@@ -2043,10 +2038,10 @@
         <v>21</v>
       </c>
       <c r="P5" s="3" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
       <c r="Q5" s="3" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="R5" s="4" t="n">
         <f aca="false">TRUE()</f>
@@ -2059,28 +2054,28 @@
         <v>6</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C6" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="G6" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="F6" s="3" t="s">
-        <v>159</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>151</v>
-      </c>
       <c r="H6" s="3" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="N6" s="3" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="O6" s="3" t="s">
         <v>50</v>
       </c>
       <c r="Q6" s="3" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="R6" s="4" t="n">
         <f aca="false">TRUE()</f>
@@ -2093,25 +2088,25 @@
         <v>7</v>
       </c>
       <c r="B7" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="F7" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>161</v>
-      </c>
-      <c r="F7" s="3" t="s">
+      <c r="G7" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="H7" s="3" t="s">
         <v>150</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>152</v>
       </c>
       <c r="O7" s="3" t="s">
         <v>50</v>
       </c>
       <c r="Q7" s="3" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="R7" s="4" t="n">
         <f aca="false">TRUE()</f>
@@ -2124,16 +2119,16 @@
         <v>8</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="O8" s="3" t="s">
         <v>21</v>
       </c>
       <c r="P8" s="3" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="R8" s="4" t="n">
         <f aca="false">TRUE()</f>
@@ -2145,25 +2140,25 @@
         <v>9</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>35</v>
       </c>
       <c r="F9" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="H9" s="3" t="s">
         <v>150</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>164</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>152</v>
       </c>
       <c r="O9" s="3" t="s">
         <v>50</v>
       </c>
       <c r="Q9" s="3" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="R9" s="4" t="n">
         <f aca="false">TRUE()</f>
@@ -2176,28 +2171,28 @@
         <v>11</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>21</v>
       </c>
       <c r="F10" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="H10" s="3" t="s">
         <v>150</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>152</v>
       </c>
       <c r="O10" s="3" t="s">
         <v>21</v>
       </c>
       <c r="Q10" s="3" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="R10" s="4" t="n">
         <f aca="false">TRUE()</f>
@@ -2209,7 +2204,7 @@
         <v>2</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C11" s="3" t="n">
         <v>40</v>
@@ -2218,16 +2213,16 @@
         <v>21</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
       <c r="L11" s="3"/>
       <c r="Q11" s="3" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="R11" s="4" t="n">
         <f aca="false">TRUE()</f>

</xml_diff>

<commit_message>
validation dataset - is now fixed for each project
</commit_message>
<xml_diff>
--- a/configurations/experiment_configs_liver.xlsx
+++ b/configurations/experiment_configs_liver.xlsx
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="295" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="162">
   <si>
     <t xml:space="preserve">var_name</t>
   </si>
@@ -268,9 +268,6 @@
   </si>
   <si>
     <t xml:space="preserve">ds_type</t>
-  </si>
-  <si>
-    <t xml:space="preserve">plan_train</t>
   </si>
   <si>
     <t xml:space="preserve">plan_valid</t>
@@ -1153,7 +1150,7 @@
   <dimension ref="A1:K1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
+      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1347,21 +1344,14 @@
       <c r="E12" s="3" t="n">
         <v>11</v>
       </c>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="3" t="s">
+      <c r="G12" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="E13" s="3" t="n">
-        <v>11</v>
-      </c>
-      <c r="G13" s="3" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="3"/>
-    </row>
+    </row>
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B26" s="3"/>
+    </row>
+    <row r="1048573" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048574" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -1403,13 +1393,13 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>84</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>85</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>4</v>
@@ -1420,114 +1410,114 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B2" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="B2" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>88</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>89</v>
       </c>
       <c r="F2" s="3" t="n">
         <v>0.1</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B3" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>91</v>
-      </c>
-      <c r="B3" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>92</v>
       </c>
       <c r="F3" s="3" t="n">
         <v>0.1</v>
       </c>
       <c r="G3" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="H3" s="3" t="s">
         <v>93</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>94</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B4" s="3" t="n">
         <v>1</v>
       </c>
       <c r="C4" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>88</v>
-      </c>
       <c r="E4" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F4" s="3" t="n">
         <v>0.1</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B5" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>96</v>
-      </c>
-      <c r="B5" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>97</v>
       </c>
       <c r="F5" s="3" t="n">
         <v>0.1</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="B6" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="B6" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="C6" s="3" t="s">
+      <c r="D6" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>100</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>101</v>
       </c>
       <c r="F6" s="3" t="n">
         <v>0.1</v>
@@ -1538,53 +1528,53 @@
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B7" s="3" t="n">
         <v>0</v>
       </c>
       <c r="C7" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>87</v>
       </c>
-      <c r="D7" s="3" t="s">
-        <v>88</v>
-      </c>
       <c r="E7" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="F7" s="3" t="n">
         <v>0.1</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="B8" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="E8" s="3" t="s">
         <v>103</v>
-      </c>
-      <c r="B8" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>104</v>
       </c>
       <c r="F8" s="3" t="n">
         <v>0.1</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B9" s="3" t="n">
         <v>0</v>
@@ -1593,7 +1583,7 @@
         <v>12</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>20</v>
@@ -1650,32 +1640,32 @@
         <v>4</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>109</v>
-      </c>
-      <c r="D2" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="C3" s="3" t="s">
         <v>112</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>113</v>
       </c>
       <c r="D3" s="3" t="n">
         <v>0</v>
@@ -1684,29 +1674,29 @@
         <v>35</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="D4" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>115</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="D4" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="D5" s="3" t="n">
         <v>0</v>
@@ -1717,13 +1707,13 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>119</v>
-      </c>
       <c r="C6" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D6" s="3" t="n">
         <v>0</v>
@@ -1773,12 +1763,12 @@
         <v>4</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D2" s="3" t="n">
         <v>0</v>
@@ -1786,7 +1776,7 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>21</v>
@@ -1794,7 +1784,7 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D4" s="3" t="n">
         <v>0</v>
@@ -1805,18 +1795,18 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="D5" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>124</v>
-      </c>
-      <c r="D5" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D6" s="3" t="n">
         <v>0</v>
@@ -1844,7 +1834,7 @@
   <dimension ref="A1:Y1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K6" activeCellId="0" sqref="K6"/>
+      <selection pane="topLeft" activeCell="G3" activeCellId="0" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="18.7578125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1857,61 +1847,61 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>144</v>
-      </c>
-      <c r="S1" s="2" t="s">
-        <v>145</v>
       </c>
       <c r="T1" s="2" t="s">
         <v>4</v>
@@ -1937,28 +1927,28 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>146</v>
-      </c>
-      <c r="C2" s="3" t="s">
-        <v>147</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>21</v>
       </c>
       <c r="F2" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="H2" s="3" t="s">
         <v>149</v>
-      </c>
-      <c r="H2" s="3" t="s">
-        <v>150</v>
       </c>
       <c r="O2" s="3" t="s">
         <v>50</v>
       </c>
       <c r="Q2" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="R2" s="4" t="n">
         <f aca="false">TRUE()</f>
@@ -1970,16 +1960,22 @@
         <v>3</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>149</v>
       </c>
       <c r="O3" s="3" t="s">
         <v>50</v>
       </c>
       <c r="Q3" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="R3" s="4" t="n">
         <f aca="false">TRUE()</f>
@@ -1992,25 +1988,25 @@
         <v>4</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>77</v>
       </c>
       <c r="F4" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="G4" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="H4" s="3" t="s">
         <v>149</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>150</v>
       </c>
       <c r="O4" s="3" t="s">
         <v>50</v>
       </c>
       <c r="Q4" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="R4" s="4" t="n">
         <f aca="false">TRUE()</f>
@@ -2023,13 +2019,13 @@
         <v>5</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F5" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="I5" s="3" t="s">
         <v>154</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>155</v>
       </c>
       <c r="J5" s="3"/>
       <c r="K5" s="3"/>
@@ -2038,10 +2034,10 @@
         <v>21</v>
       </c>
       <c r="P5" s="3" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="Q5" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="R5" s="4" t="n">
         <f aca="false">TRUE()</f>
@@ -2054,28 +2050,28 @@
         <v>6</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>147</v>
-      </c>
       <c r="F6" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="N6" s="3" t="s">
         <v>157</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="N6" s="3" t="s">
-        <v>158</v>
       </c>
       <c r="O6" s="3" t="s">
         <v>50</v>
       </c>
       <c r="Q6" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="R6" s="4" t="n">
         <f aca="false">TRUE()</f>
@@ -2088,25 +2084,25 @@
         <v>7</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F7" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="G7" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="G7" s="3" t="s">
+      <c r="H7" s="3" t="s">
         <v>149</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>150</v>
       </c>
       <c r="O7" s="3" t="s">
         <v>50</v>
       </c>
       <c r="Q7" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="R7" s="4" t="n">
         <f aca="false">TRUE()</f>
@@ -2119,16 +2115,16 @@
         <v>8</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="O8" s="3" t="s">
         <v>21</v>
       </c>
       <c r="P8" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="R8" s="4" t="n">
         <f aca="false">TRUE()</f>
@@ -2140,25 +2136,25 @@
         <v>9</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>35</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="O9" s="3" t="s">
         <v>50</v>
       </c>
       <c r="Q9" s="3" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="R9" s="4" t="n">
         <f aca="false">TRUE()</f>
@@ -2171,28 +2167,28 @@
         <v>11</v>
       </c>
       <c r="B10" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>146</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>147</v>
       </c>
       <c r="D10" s="3" t="s">
         <v>21</v>
       </c>
       <c r="F10" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="G10" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="G10" s="3" t="s">
+      <c r="H10" s="3" t="s">
         <v>149</v>
-      </c>
-      <c r="H10" s="3" t="s">
-        <v>150</v>
       </c>
       <c r="O10" s="3" t="s">
         <v>21</v>
       </c>
       <c r="Q10" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="R10" s="4" t="n">
         <f aca="false">TRUE()</f>
@@ -2204,7 +2200,7 @@
         <v>2</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C11" s="3" t="n">
         <v>40</v>
@@ -2213,16 +2209,16 @@
         <v>21</v>
       </c>
       <c r="F11" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="I11" s="3" t="s">
         <v>154</v>
-      </c>
-      <c r="I11" s="3" t="s">
-        <v>155</v>
       </c>
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
       <c r="L11" s="3"/>
       <c r="Q11" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="R11" s="4" t="n">
         <f aca="false">TRUE()</f>

</xml_diff>

<commit_message>
Now setting ray tune
</commit_message>
<xml_diff>
--- a/configurations/experiment_configs_liver.xlsx
+++ b/configurations/experiment_configs_liver.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="model_params" sheetId="1" state="visible" r:id="rId3"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="162">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="161">
   <si>
     <t xml:space="preserve">var_name</t>
   </si>
@@ -54,145 +54,142 @@
     <t xml:space="preserve">Unnamed: 8</t>
   </si>
   <si>
+    <t xml:space="preserve">arch</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[ResidualUNet3D,UNet3D,VTUNet, nnUNet,SwinUNETR,DynUNet]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">choice</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nnUNet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SwinUNETR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DynUNet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">base_ch_opts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[16,32]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rrr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">depth_opts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[4,6]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">qrandint</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">optimizer</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Adam</t>
+  </si>
+  <si>
+    <t xml:space="preserve">lr</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[1e-2,5e-4]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">qloguniform</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.001</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.0005</t>
+  </si>
+  <si>
+    <t xml:space="preserve">one_cycle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[True,False]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mom_low</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.6,0.9]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">spec</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.85</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mom_added</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0.5,0.25]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">heavy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">layer_order</t>
+  </si>
+  <si>
+    <t xml:space="preserve">clb</t>
+  </si>
+  <si>
+    <t xml:space="preserve">in_channels</t>
+  </si>
+  <si>
+    <t xml:space="preserve">n_bottlenecks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[0,4]</t>
+  </si>
+  <si>
+    <t xml:space="preserve">randint</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">tune_region_id</t>
+  </si>
+  <si>
+    <t xml:space="preserve">deep_supervision</t>
+  </si>
+  <si>
+    <t xml:space="preserve">self_attention</t>
+  </si>
+  <si>
+    <t xml:space="preserve">compiled</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unnamed: 5</t>
+  </si>
+  <si>
     <t xml:space="preserve">Unnamed: 9</t>
-  </si>
-  <si>
-    <t xml:space="preserve">base_ch_opts</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[16,32]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">choice</t>
-  </si>
-  <si>
-    <t xml:space="preserve">rrr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">lr</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[1e-4,5e-2]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">qloguniform</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.001</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.0005</t>
-  </si>
-  <si>
-    <t xml:space="preserve">deep_supervision</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[True,False]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">arch</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[ResidualUNet3D,UNet3D,VTUNet, nnUNet,SwinUNETR,DynUNet]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nnUNet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SwinUNETR</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DynUNet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.5D</t>
-  </si>
-  <si>
-    <t xml:space="preserve">depth_opts</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[4,6]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">qrandint</t>
-  </si>
-  <si>
-    <t xml:space="preserve">5</t>
-  </si>
-  <si>
-    <t xml:space="preserve">optimizer</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Adam</t>
-  </si>
-  <si>
-    <t xml:space="preserve">one_cycle</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mom_low</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.6,0.9]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">spec</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.85</t>
-  </si>
-  <si>
-    <t xml:space="preserve">mom_added</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0.5,0.25]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">heavy</t>
-  </si>
-  <si>
-    <t xml:space="preserve">layer_order</t>
-  </si>
-  <si>
-    <t xml:space="preserve">clb</t>
-  </si>
-  <si>
-    <t xml:space="preserve">in_channels</t>
-  </si>
-  <si>
-    <t xml:space="preserve">n_bottlenecks</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[0,4]</t>
-  </si>
-  <si>
-    <t xml:space="preserve">randint</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">4</t>
-  </si>
-  <si>
-    <t xml:space="preserve">tune_region_id</t>
-  </si>
-  <si>
-    <t xml:space="preserve">self_attention</t>
-  </si>
-  <si>
-    <t xml:space="preserve">compiled</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Unnamed: 5</t>
   </si>
   <si>
     <t xml:space="preserve">Unnamed: 10</t>
@@ -814,17 +811,16 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J17"/>
+  <dimension ref="A1:I17"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D4" activeCellId="0" sqref="D4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E23" activeCellId="0" sqref="E23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.16015625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="20.09"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="47.91"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="3" style="1" width="20.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="1" style="1" width="17.66"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="6" style="0" width="8.59"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -855,36 +851,45 @@
       <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
-        <v>9</v>
-      </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="C2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="E2" s="3" t="s">
+      <c r="F2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>13</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>12</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="D3" s="3" t="n">
         <v>1</v>
@@ -892,36 +897,30 @@
       <c r="E3" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F3" s="3" t="s">
-        <v>18</v>
-      </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="C4" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>12</v>
-      </c>
       <c r="D4" s="3" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>21</v>
       </c>
+      <c r="F4" s="3" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B5" s="3" t="s">
         <v>23</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>12</v>
       </c>
       <c r="D5" s="3" t="n">
         <v>0</v>
@@ -929,79 +928,70 @@
       <c r="E5" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="F5" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="J5" s="3" t="s">
-        <v>27</v>
-      </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="F6" s="3" t="s">
         <v>29</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D6" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" s="3" t="s">
         <v>32</v>
-      </c>
-      <c r="D7" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>20</v>
-      </c>
       <c r="C8" s="3" t="s">
-        <v>12</v>
+        <v>35</v>
       </c>
       <c r="D8" s="3" t="n">
         <v>0</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="D9" s="3" t="n">
         <v>0</v>
@@ -1015,120 +1005,120 @@
         <v>40</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>38</v>
+        <v>11</v>
       </c>
       <c r="D10" s="3" t="n">
         <v>0</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>42</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>12</v>
+        <v>41</v>
       </c>
       <c r="D11" s="3" t="n">
         <v>0</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>35</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D12" s="3" t="n">
         <v>0</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>45</v>
+        <v>22</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C13" s="3" t="s">
         <v>46</v>
       </c>
       <c r="D13" s="3" t="n">
         <v>0</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>21</v>
+        <v>47</v>
+      </c>
+      <c r="F13" s="3" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B14" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="C14" s="3" t="s">
         <v>49</v>
       </c>
       <c r="D14" s="3" t="n">
         <v>0</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="F14" s="3" t="s">
-        <v>51</v>
+        <v>22</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>11</v>
       </c>
       <c r="D15" s="3" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D16" s="3" t="n">
         <v>0</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="3" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D17" s="3" t="n">
         <v>0</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1149,8 +1139,8 @@
   </sheetPr>
   <dimension ref="A1:K1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A12" activeCellId="0" sqref="A12"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J32" activeCellId="0" sqref="J32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.59765625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1177,7 +1167,7 @@
         <v>4</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>6</v>
@@ -1189,29 +1179,29 @@
         <v>8</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>9</v>
+        <v>54</v>
       </c>
       <c r="K1" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D2" s="1" t="n">
+        <v>1</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="G2" s="3" t="s">
         <v>57</v>
-      </c>
-      <c r="D2" s="1" t="n">
-        <v>1</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="G2" s="3" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B3" s="3"/>
       <c r="D3" s="1" t="n">
@@ -1224,7 +1214,7 @@
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D4" s="1" t="n">
         <v>1</v>
@@ -1233,27 +1223,27 @@
         <v>128</v>
       </c>
       <c r="F4" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="G4" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="H4" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="I4" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="J4" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="J4" s="3" t="s">
+      <c r="K4" s="3" t="s">
         <v>65</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="D5" s="3" t="n">
         <v>0</v>
@@ -1264,88 +1254,88 @@
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="C6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="D6" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="E6" s="3" t="s">
+      <c r="I6" s="3" t="s">
         <v>70</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D7" s="3" t="n">
         <v>0</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="D8" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" s="3" t="s">
         <v>74</v>
-      </c>
-      <c r="D8" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="E9" s="3" t="s">
         <v>76</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="B10" s="3" t="s">
-        <v>79</v>
-      </c>
       <c r="E10" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E12" s="3" t="n">
         <v>11</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1393,13 +1383,13 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>83</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>84</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>4</v>
@@ -1410,189 +1400,189 @@
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="B2" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>85</v>
       </c>
-      <c r="B2" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>87</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>88</v>
       </c>
       <c r="F2" s="3" t="n">
         <v>0.1</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B3" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="E3" s="3" t="s">
         <v>90</v>
-      </c>
-      <c r="B3" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>91</v>
       </c>
       <c r="F3" s="3" t="n">
         <v>0.1</v>
       </c>
       <c r="G3" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="H3" s="3" t="s">
         <v>92</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>93</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B4" s="3" t="n">
         <v>1</v>
       </c>
       <c r="C4" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>87</v>
-      </c>
       <c r="E4" s="3" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="F4" s="3" t="n">
         <v>0.1</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B5" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>95</v>
-      </c>
-      <c r="B5" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>96</v>
       </c>
       <c r="F5" s="3" t="n">
         <v>0.1</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B6" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="B6" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="C6" s="3" t="s">
+      <c r="D6" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>99</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>100</v>
       </c>
       <c r="F6" s="3" t="n">
         <v>0.1</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B7" s="3" t="n">
         <v>0</v>
       </c>
       <c r="C7" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D7" s="3" t="s">
         <v>86</v>
       </c>
-      <c r="D7" s="3" t="s">
-        <v>87</v>
-      </c>
       <c r="E7" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F7" s="3" t="n">
         <v>0.1</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="B8" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="E8" s="3" t="s">
         <v>102</v>
-      </c>
-      <c r="B8" s="3" t="n">
-        <v>1</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>103</v>
       </c>
       <c r="F8" s="3" t="n">
         <v>0.1</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B9" s="3" t="n">
         <v>0</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>20</v>
+        <v>31</v>
       </c>
       <c r="F9" s="3" t="n">
         <v>0.1</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -1640,86 +1630,86 @@
         <v>4</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>107</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>108</v>
-      </c>
-      <c r="D2" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="C3" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="D3" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="F3" s="3" t="s">
         <v>112</v>
-      </c>
-      <c r="D3" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D4" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>114</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="D4" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="D5" s="3" t="n">
         <v>0</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>118</v>
-      </c>
       <c r="C6" s="3" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="D6" s="3" t="n">
         <v>0</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -1763,12 +1753,12 @@
         <v>4</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="3" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D2" s="3" t="n">
         <v>0</v>
@@ -1776,43 +1766,43 @@
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="3" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D4" s="3" t="n">
         <v>0</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="D5" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>123</v>
-      </c>
-      <c r="D5" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="D6" s="3" t="n">
         <v>0</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -1847,61 +1837,61 @@
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="2" t="s">
+        <v>125</v>
+      </c>
+      <c r="B1" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C1" s="2" t="s">
         <v>127</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>136</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="Q1" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="Q1" s="2" t="s">
+      <c r="R1" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="R1" s="2" t="s">
+      <c r="S1" s="2" t="s">
         <v>143</v>
-      </c>
-      <c r="S1" s="2" t="s">
-        <v>144</v>
       </c>
       <c r="T1" s="2" t="s">
         <v>4</v>
@@ -1927,28 +1917,28 @@
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="C2" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="D2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F2" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="D2" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="F2" s="3" t="s">
+      <c r="G2" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="H2" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="O2" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q2" s="3" t="s">
         <v>149</v>
-      </c>
-      <c r="O2" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="Q2" s="3" t="s">
-        <v>150</v>
       </c>
       <c r="R2" s="4" t="n">
         <f aca="false">TRUE()</f>
@@ -1960,22 +1950,22 @@
         <v>3</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="G3" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="H3" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="H3" s="3" t="s">
+      <c r="O3" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q3" s="3" t="s">
         <v>149</v>
-      </c>
-      <c r="O3" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="Q3" s="3" t="s">
-        <v>150</v>
       </c>
       <c r="R3" s="4" t="n">
         <f aca="false">TRUE()</f>
@@ -1988,25 +1978,25 @@
         <v>4</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="F4" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="G4" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="H4" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="H4" s="3" t="s">
-        <v>149</v>
-      </c>
       <c r="O4" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="Q4" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="R4" s="4" t="n">
         <f aca="false">TRUE()</f>
@@ -2019,25 +2009,25 @@
         <v>5</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F5" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="I5" s="3" t="s">
         <v>153</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>154</v>
       </c>
       <c r="J5" s="3"/>
       <c r="K5" s="3"/>
       <c r="L5" s="3"/>
       <c r="O5" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="P5" s="3" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="Q5" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="R5" s="4" t="n">
         <f aca="false">TRUE()</f>
@@ -2050,28 +2040,28 @@
         <v>6</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="C6" s="3" t="s">
-        <v>146</v>
-      </c>
       <c r="F6" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="N6" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="G6" s="3" t="s">
-        <v>148</v>
-      </c>
-      <c r="H6" s="3" t="s">
+      <c r="O6" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q6" s="3" t="s">
         <v>149</v>
-      </c>
-      <c r="N6" s="3" t="s">
-        <v>157</v>
-      </c>
-      <c r="O6" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="Q6" s="3" t="s">
-        <v>150</v>
       </c>
       <c r="R6" s="4" t="n">
         <f aca="false">TRUE()</f>
@@ -2084,25 +2074,25 @@
         <v>7</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="F7" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="G7" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="G7" s="3" t="s">
+      <c r="H7" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="H7" s="3" t="s">
+      <c r="O7" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="Q7" s="3" t="s">
         <v>149</v>
-      </c>
-      <c r="O7" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="Q7" s="3" t="s">
-        <v>150</v>
       </c>
       <c r="R7" s="4" t="n">
         <f aca="false">TRUE()</f>
@@ -2115,16 +2105,16 @@
         <v>8</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="F8" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="O8" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="P8" s="3" t="s">
         <v>159</v>
-      </c>
-      <c r="O8" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="P8" s="3" t="s">
-        <v>160</v>
       </c>
       <c r="R8" s="4" t="n">
         <f aca="false">TRUE()</f>
@@ -2136,25 +2126,25 @@
         <v>9</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="O9" s="3" t="s">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="Q9" s="3" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="R9" s="4" t="n">
         <f aca="false">TRUE()</f>
@@ -2167,28 +2157,28 @@
         <v>11</v>
       </c>
       <c r="B10" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="D10" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F10" s="3" t="s">
         <v>146</v>
       </c>
-      <c r="D10" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="F10" s="3" t="s">
+      <c r="G10" s="3" t="s">
         <v>147</v>
       </c>
-      <c r="G10" s="3" t="s">
+      <c r="H10" s="3" t="s">
         <v>148</v>
       </c>
-      <c r="H10" s="3" t="s">
+      <c r="O10" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q10" s="3" t="s">
         <v>149</v>
-      </c>
-      <c r="O10" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="Q10" s="3" t="s">
-        <v>150</v>
       </c>
       <c r="R10" s="4" t="n">
         <f aca="false">TRUE()</f>
@@ -2200,25 +2190,25 @@
         <v>2</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C11" s="3" t="n">
         <v>40</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F11" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="I11" s="3" t="s">
         <v>153</v>
-      </c>
-      <c r="I11" s="3" t="s">
-        <v>154</v>
       </c>
       <c r="J11" s="3"/>
       <c r="K11" s="3"/>
       <c r="L11" s="3"/>
       <c r="Q11" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="R11" s="4" t="n">
         <f aca="false">TRUE()</f>

</xml_diff>